<commit_message>
Modify LED part number in BOM
</commit_message>
<xml_diff>
--- a/BLM_2017 BOM - Rev. A.xlsx
+++ b/BLM_2017 BOM - Rev. A.xlsx
@@ -65,15 +65,6 @@
     <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12, D13, D14, D15, D16, D17, D18, D19, D20</t>
   </si>
   <si>
-    <t>Cree Inc.</t>
-  </si>
-  <si>
-    <t>C566C-RFS-CT0W0BB1</t>
-  </si>
-  <si>
-    <t>C566C-RFS-CT0W0BB1-ND</t>
-  </si>
-  <si>
     <t>L1, L2</t>
   </si>
   <si>
@@ -153,13 +144,22 @@
   </si>
   <si>
     <t>Supplier Subtotal</t>
+  </si>
+  <si>
+    <t>365-1546-1-ND</t>
+  </si>
+  <si>
+    <t>OVS5MRBCR4</t>
+  </si>
+  <si>
+    <t>TT Electronics/Optek Technology</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +179,13 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -222,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -230,6 +237,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +520,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -535,33 +545,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -593,7 +603,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -625,16 +635,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>42</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="E4" s="3">
         <v>20</v>
@@ -646,27 +656,27 @@
         <v>7</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I4" s="3">
-        <v>0.32</v>
+        <v>0.63</v>
       </c>
       <c r="J4" s="3">
-        <v>6.4</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
@@ -678,7 +688,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I5" s="3">
         <v>0.53</v>
@@ -689,16 +699,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
@@ -710,7 +720,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I6" s="3">
         <v>0.15</v>
@@ -721,16 +731,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3">
         <v>2</v>
@@ -742,7 +752,7 @@
         <v>7</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I7" s="3">
         <v>0.15</v>
@@ -753,16 +763,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -774,7 +784,7 @@
         <v>7</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I8" s="3">
         <v>6.17</v>
@@ -786,7 +796,7 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J9" s="4">
         <f>SUM(J2:J8)</f>
-        <v>14.940000000000001</v>
+        <v>21.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[BOM] Update bill of materials
- Replace feedback resistors
</commit_message>
<xml_diff>
--- a/BLM_2017 BOM - Rev. A.xlsx
+++ b/BLM_2017 BOM - Rev. A.xlsx
@@ -92,12 +92,6 @@
     <t>R2, R3</t>
   </si>
   <si>
-    <t>ERJ-3EKF10R0V</t>
-  </si>
-  <si>
-    <t>P10.0HCT-ND</t>
-  </si>
-  <si>
     <t>2-Channel Step-Up LED Driver</t>
   </si>
   <si>
@@ -153,6 +147,12 @@
   </si>
   <si>
     <t>TT Electronics/Optek Technology</t>
+  </si>
+  <si>
+    <t>P3.3AJCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-3RQF3R3V</t>
   </si>
 </sst>
 </file>
@@ -520,9 +520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -545,33 +543,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -603,7 +601,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -635,16 +633,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E4" s="3">
         <v>20</v>
@@ -656,7 +654,7 @@
         <v>7</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I4" s="3">
         <v>0.63</v>
@@ -667,7 +665,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
@@ -699,7 +697,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>17</v>
@@ -731,7 +729,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>21</v>
@@ -740,7 +738,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E7" s="3">
         <v>2</v>
@@ -752,27 +750,27 @@
         <v>7</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="I7" s="3">
-        <v>0.15</v>
+        <v>0.42</v>
       </c>
       <c r="J7" s="3">
-        <v>0.3</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -784,7 +782,7 @@
         <v>7</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I8" s="3">
         <v>6.17</v>
@@ -796,7 +794,7 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J9" s="4">
         <f>SUM(J2:J8)</f>
-        <v>21.14</v>
+        <v>21.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>